<commit_message>
fix: change leadtime to leadTimeHour for NORA3 to reuse more arguments across package
</commit_message>
<xml_diff>
--- a/.github/ArgumentUsage.xlsx
+++ b/.github/ArgumentUsage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/erikkus_cicero_oslo_no/Documents/Documents/31569 - ClimHub/ClimHub_GitHub/.github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{1892F552-129D-4505-A1EB-B37419729DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53390E1-26EE-4588-9D22-047D65AB0AE2}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{1892F552-129D-4505-A1EB-B37419729DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F55AAC-3F36-4DC4-8BB1-A5CBCBE1C000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7ED2EDC4-BD5E-49E4-AE72-BC07D1D41013}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="153">
   <si>
     <t>Argument</t>
   </si>
@@ -71,9 +71,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>write</t>
-  </si>
-  <si>
     <t>compression</t>
   </si>
   <si>
@@ -450,13 +447,61 @@
   </si>
   <si>
     <t>closeConnections</t>
+  </si>
+  <si>
+    <t>What variable to obtain data for</t>
+  </si>
+  <si>
+    <t>What model to obtain data for</t>
+  </si>
+  <si>
+    <t>What scenario to obtain data for</t>
+  </si>
+  <si>
+    <t>Start of time window for data access</t>
+  </si>
+  <si>
+    <t>Stop of time window for data access</t>
+  </si>
+  <si>
+    <t>Whether to remove temporary files or not</t>
+  </si>
+  <si>
+    <t>lead time of data to access</t>
+  </si>
+  <si>
+    <t>whether to close connections at end of function</t>
+  </si>
+  <si>
+    <t>what time zone time window is specified in</t>
+  </si>
+  <si>
+    <t>what product type to query data from</t>
+  </si>
+  <si>
+    <t>what data type to query data from</t>
+  </si>
+  <si>
+    <t>what soil layer to query data from</t>
+  </si>
+  <si>
+    <t>what level to query data from</t>
+  </si>
+  <si>
+    <t>Access_KlimaiNorge2100</t>
+  </si>
+  <si>
+    <t>Access_NORA3</t>
+  </si>
+  <si>
+    <t>Access_reanalysis_cerra_single_levels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,12 +520,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -505,16 +544,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,20 +885,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92B5E-1B5B-4594-8844-F2047C5EAE1B}">
-  <dimension ref="A1:AA64"/>
+  <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="2" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -870,111 +906,120 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="Q1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -982,654 +1027,770 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="V3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" t="s">
-        <v>18</v>
-      </c>
-      <c r="X10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="G17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="L20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="L21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="I22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="M24" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="J25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="L26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="N26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="K27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
       </c>
-      <c r="K28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="K29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="P29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
-      </c>
-      <c r="M30" t="s">
-        <v>18</v>
-      </c>
-      <c r="N30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="N31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="R31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="O32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="S32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="P33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
-      </c>
-      <c r="P34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="T34" t="s">
+        <v>17</v>
+      </c>
+      <c r="W34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="T35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="W35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>18</v>
-      </c>
-      <c r="T36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="U36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="R37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="U37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="R38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="U38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="R39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="V39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
-      </c>
-      <c r="S40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="V40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="V41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B41" t="s">
-        <v>102</v>
-      </c>
-      <c r="S41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="S42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="W42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
-      </c>
-      <c r="T43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="X43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
-      </c>
-      <c r="U44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
-      </c>
-      <c r="V45" t="s">
-        <v>18</v>
-      </c>
-      <c r="W45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B46" t="s">
         <v>116</v>
       </c>
-      <c r="X46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B47" t="s">
         <v>117</v>
       </c>
-      <c r="X47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
-      </c>
-      <c r="X48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>148</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>137</v>
+      <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>